<commit_message>
DB schema for G30
</commit_message>
<xml_diff>
--- a/G30/DB_Schema_Design.xlsx
+++ b/G30/DB_Schema_Design.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Chitkara\G30\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D633B327-E145-474E-841C-33F8831DF314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3126C8D-43F8-4475-B048-0996E69F81EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{369902F8-6569-497F-B003-95CBCFF59226}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{369902F8-6569-497F-B003-95CBCFF59226}"/>
   </bookViews>
   <sheets>
     <sheet name="product_management" sheetId="1" r:id="rId1"/>
+    <sheet name="user_management" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="66">
   <si>
     <t>Table</t>
   </si>
@@ -160,13 +161,85 @@
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>registered_on</t>
+  </si>
+  <si>
+    <t>varchar(30)</t>
+  </si>
+  <si>
+    <t>char(10)</t>
+  </si>
+  <si>
+    <t>user_address</t>
+  </si>
+  <si>
+    <t>primary_address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>pin</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>char(6)</t>
+  </si>
+  <si>
+    <t>varchar(20) Default- "India"</t>
+  </si>
+  <si>
+    <t>Master_city</t>
+  </si>
+  <si>
+    <t>city_name</t>
+  </si>
+  <si>
+    <t>state_id</t>
+  </si>
+  <si>
+    <t>Master_state</t>
+  </si>
+  <si>
+    <t>state_name</t>
+  </si>
+  <si>
+    <t>updated_on</t>
+  </si>
+  <si>
+    <t>updated_by</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,6 +251,28 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,11 +330,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -983,7 +1082,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
+      <xdr:colOff>171450</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
@@ -1523,7 +1622,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>413658</xdr:colOff>
+      <xdr:colOff>267608</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>37192</xdr:rowOff>
     </xdr:to>
@@ -1673,7 +1772,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>379790</xdr:colOff>
+      <xdr:colOff>233740</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>153609</xdr:rowOff>
     </xdr:to>
@@ -1817,6 +1916,463 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>830580</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CAD9D2D-D3C1-5967-6721-D72C4F9F27FC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2225040" y="403860"/>
+          <a:ext cx="1813560" cy="205740"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="525780" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15FCA4E3-ECE2-807F-790B-EDDBB183B8AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="419100"/>
+          <a:ext cx="525780" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="1"/>
+            <a:t>1:M</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1478280</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D4C394C-A73A-7C9B-90EA-B3C7D7D5844E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6774180" y="1478280"/>
+          <a:ext cx="1219200" cy="937260"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1729740</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="8" name="Straight Arrow Connector 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBDA67A3-D4D2-5E3B-58B8-19F3E3D62269}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7025640" y="358140"/>
+          <a:ext cx="3299460" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Arrow Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA028FAD-0BEF-7DC1-849B-7D43B2464FD2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="8313420" y="571500"/>
+          <a:ext cx="2026920" cy="1851660"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="365421" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="TextBox 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75773A1D-0692-D194-2818-03C78B0C270D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8321040" y="632460"/>
+          <a:ext cx="365421" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="1"/>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2042160</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="365421" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="TextBox 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F3BC72D-8511-42F9-A131-916DDA1052B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7338060" y="1950720"/>
+          <a:ext cx="365421" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="1"/>
+            <a:t>1:1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>205740</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="571500" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="TextBox 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E2D0A91-A348-47BA-ADCF-AE443BB53CDD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9090660" y="1371600"/>
+          <a:ext cx="571500" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100" b="1"/>
+            <a:t>1:M</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2119,8 +2675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA7D8B4-E9DE-41FB-A9A5-788896FE6B20}">
   <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2132,7 +2688,7 @@
     <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
@@ -2331,8 +2887,12 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="I10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="M10" s="2" t="s">
         <v>34</v>
       </c>
@@ -2387,4 +2947,243 @@
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1BA3D0-DE68-42EF-8997-F6D71EE416F7}">
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.88671875" style="4"/>
+    <col min="5" max="5" width="18.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="4"/>
+    <col min="8" max="8" width="13.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H12" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H14" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="H15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>